<commit_message>
Final Uploading of re-labelled parcel and parcellation data.
</commit_message>
<xml_diff>
--- a/Review/John/LUC_codes/LUC_codeToName.xlsx
+++ b/Review/John/LUC_codes/LUC_codeToName.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/758d8064f70bcc3d/Desktop/DSPG/2022_DSPG_landuse/LUC_codes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/758d8064f70bcc3d/Desktop/DSPG/2022_DSPG_landuse/Review/John/LUC_codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="8_{737372F7-7496-49EB-8BF2-7FC2B285B619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFC647FF-640E-4976-94FC-9466E80C8ADE}"/>
+  <xr:revisionPtr revIDLastSave="269" documentId="8_{737372F7-7496-49EB-8BF2-7FC2B285B619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CF13464-325C-4F62-A790-3FD78E98D747}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{9A705C74-2FAC-43FA-AA72-2044838330E2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{9A705C74-2FAC-43FA-AA72-2044838330E2}"/>
   </bookViews>
   <sheets>
     <sheet name="codeToName" sheetId="1" r:id="rId1"/>
     <sheet name="Powhatan" sheetId="2" r:id="rId2"/>
-    <sheet name="Goochland 2018" sheetId="3" r:id="rId3"/>
-    <sheet name="Goochland 2022" sheetId="4" r:id="rId4"/>
-    <sheet name="Goochland Parcellation 2018" sheetId="5" r:id="rId5"/>
-    <sheet name="Goochland Parcellation 2022" sheetId="6" r:id="rId6"/>
+    <sheet name="Goochland" sheetId="7" r:id="rId3"/>
+    <sheet name="Goochland 2018" sheetId="3" r:id="rId4"/>
+    <sheet name="Goochland 2022" sheetId="4" r:id="rId5"/>
+    <sheet name="Goochland Parcellation 2018" sheetId="5" r:id="rId6"/>
+    <sheet name="Goochland Parcellation 2022" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>Single Family Residential Urban</t>
   </si>
@@ -274,6 +275,30 @@
   </si>
   <si>
     <t>Undefined</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>comm/ind</t>
+  </si>
+  <si>
+    <t>res sub</t>
+  </si>
+  <si>
+    <t>ag20-100</t>
+  </si>
+  <si>
+    <t>ag100+</t>
+  </si>
+  <si>
+    <t>res urb</t>
+  </si>
+  <si>
+    <t>multi</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -637,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E15F759-A0BE-468C-88EE-28D036106ECE}">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -856,6 +881,97 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC32DEF-0BBF-47BC-80D1-34F2D2AEE5BA}">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="22.59765625" customWidth="1"/>
+    <col min="3" max="3" width="22.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C5073D-71E7-43A2-8DD3-B326BDE49DC2}">
   <dimension ref="B2:C29"/>
   <sheetViews>
@@ -1098,7 +1214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92471D1B-564B-4A89-A1D2-10658B5B4434}">
   <dimension ref="B2:C27"/>
   <sheetViews>
@@ -1324,7 +1440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2351B56F-DC44-4109-95B5-BA5E68101635}">
   <dimension ref="B2:C13"/>
   <sheetViews>
@@ -1438,7 +1554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567E671B-4990-41EB-9132-172A0614D27D}">
   <dimension ref="B2:C16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updating error in relabeling.
</commit_message>
<xml_diff>
--- a/Review/John/LUC_codes/LUC_codeToName.xlsx
+++ b/Review/John/LUC_codes/LUC_codeToName.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/758d8064f70bcc3d/Desktop/DSPG/2022_DSPG_landuse/Review/John/LUC_codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="8_{737372F7-7496-49EB-8BF2-7FC2B285B619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CF13464-325C-4F62-A790-3FD78E98D747}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="8_{737372F7-7496-49EB-8BF2-7FC2B285B619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCF29E24-889F-49B5-B199-863844744F5A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{9A705C74-2FAC-43FA-AA72-2044838330E2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{9A705C74-2FAC-43FA-AA72-2044838330E2}"/>
   </bookViews>
   <sheets>
     <sheet name="codeToName" sheetId="1" r:id="rId1"/>
@@ -663,7 +663,7 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C386F9CA-D3ED-42A9-9F1D-1EC60B56B0C4}">
   <dimension ref="B2:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -884,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC32DEF-0BBF-47BC-80D1-34F2D2AEE5BA}">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>